<commit_message>
Update Programs ranking based on no. of beneficiaries & expenditure.xlsx
</commit_message>
<xml_diff>
--- a/05 clean data/Programs ranking based on no. of beneficiaries & expenditure.xlsx
+++ b/05 clean data/Programs ranking based on no. of beneficiaries & expenditure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qixue/Documents/GitHub/WB-Social-Protection-Capstone/05 clean data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC1E501-3CDD-7B4D-A749-1735DA332551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C51DE7A-B687-8E47-8B7B-CFC27699D4CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5120" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{688F82F1-2EB9-5F4F-BB06-44294B8C23A7}"/>
+    <workbookView xWindow="-5120" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{688F82F1-2EB9-5F4F-BB06-44294B8C23A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Rationale" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Philippines</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>Ukraine</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
   </si>
   <si>
     <t>Tulong Panghanapbuhay sa Ating Displace/Disadvantaged Workers Program (DOLE) Second Tranche</t>
-  </si>
-  <si>
-    <t>Unemployment social assistance</t>
   </si>
   <si>
     <t>Auxilio Emergencial 1 (AE1)</t>
@@ -698,8 +692,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06AC7203-2AB1-5249-8659-E712EFCBA10A}" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C6" xr:uid="{EE44B335-1DF0-E74A-A334-0D93B0385DA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06AC7203-2AB1-5249-8659-E712EFCBA10A}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C5" xr:uid="{EE44B335-1DF0-E74A-A334-0D93B0385DA5}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BA4CEEF3-E7AE-B444-BA2B-A815D982E8C0}" name="Country Name" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{253FBFF2-3930-FA49-91A0-B256BE274CDB}" name="Program Name" dataDxfId="6"/>
@@ -1034,7 +1028,7 @@
     <row r="2" spans="2:4" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="14"/>
@@ -1046,21 +1040,21 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
@@ -1082,41 +1076,41 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
     </row>
     <row r="12" spans="2:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1135,7 +1129,7 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -1149,13 +1143,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4">
         <v>84600000</v>
@@ -1174,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4">
         <v>15000000</v>
@@ -1185,7 +1179,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4">
         <v>6830000</v>
@@ -1196,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4">
         <v>6000000</v>
@@ -1215,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4">
         <v>863667</v>
@@ -1223,10 +1217,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4">
         <v>341600</v>
@@ -1237,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4">
         <v>337198</v>
@@ -1245,10 +1239,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
         <v>248282</v>
@@ -1256,10 +1250,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
         <v>200000</v>
@@ -1267,7 +1261,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4">
         <v>86000</v>
@@ -1275,7 +1269,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4">
         <v>82000</v>
@@ -1283,10 +1277,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4">
         <v>75000</v>
@@ -1294,10 +1288,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4">
         <v>30000</v>
@@ -1316,10 +1310,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1332,13 +1326,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="8">
         <v>82720000</v>
@@ -1357,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="8">
         <v>15000000</v>
@@ -1368,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="8">
         <v>2600000</v>
@@ -1376,23 +1370,12 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8">
-        <v>2300000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="8">
         <v>797222</v>
       </c>
     </row>
@@ -1412,7 +1395,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1425,21 +1408,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7">
         <v>11120000000</v>
@@ -1455,10 +1438,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="7">
         <v>192400000</v>
@@ -1466,10 +1449,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="7">
         <v>68000000</v>
@@ -1477,10 +1460,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7">
         <v>57000000</v>
@@ -1488,10 +1471,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="7">
         <v>47300000</v>
@@ -1499,10 +1482,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7">
         <v>34400000</v>
@@ -1510,10 +1493,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7">
         <v>13900000</v>
@@ -1521,7 +1504,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7">
         <v>6222222.2000000002</v>
@@ -1529,10 +1512,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="7">
         <v>4000000</v>
@@ -1540,10 +1523,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7">
         <v>1950000</v>
@@ -1564,7 +1547,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1578,21 +1561,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7">
         <v>263400000</v>

</xml_diff>